<commit_message>
Removing products from the cart
</commit_message>
<xml_diff>
--- a/Ivan Mitrev/5.4.19/Test Case Ivan Mitrev.xlsx
+++ b/Ivan Mitrev/5.4.19/Test Case Ivan Mitrev.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\12345\SoftwareTesting2201\Ivan Mitrev\5.4.19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DF5295-0183-4AE1-BE9B-71BC9403663D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23FD3FC-81CC-4DD3-970F-551278178017}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,9 +59,6 @@
 Website: http://skillo-bg.com</t>
   </si>
   <si>
-    <t>open URL to online store</t>
-  </si>
-  <si>
     <t>IM</t>
   </si>
   <si>
@@ -69,6 +66,9 @@
   </si>
   <si>
     <t>1. The user see site for online store</t>
+  </si>
+  <si>
+    <t>open Home page to Online store</t>
   </si>
 </sst>
 </file>
@@ -144,15 +144,6 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -164,6 +155,15 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,7 +555,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,24 +567,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
     </row>
@@ -592,15 +592,15 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>12</v>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="2">
         <v>1</v>
       </c>
     </row>
@@ -608,25 +608,25 @@
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="5">
         <v>43501</v>
       </c>
     </row>
@@ -634,15 +634,15 @@
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>13</v>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="6"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -653,24 +653,24 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>